<commit_message>
minor bugfixes on web page
</commit_message>
<xml_diff>
--- a/data/teams_db.xlsx
+++ b/data/teams_db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbrav\BravoRanking\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5892134-20D0-4BE9-A471-90328E6CAB4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA4EDF5-E64A-421A-A891-F3F3CA838517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1585" uniqueCount="880">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1587" uniqueCount="880">
   <si>
     <t>team</t>
   </si>
@@ -2833,7 +2833,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E0B0BB44-9E7E-43A7-AA99-FFF6C6318EC7}" name="Tableau1" displayName="Tableau1" ref="A1:K369" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:K369" xr:uid="{E0B0BB44-9E7E-43A7-AA99-FFF6C6318EC7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K369">
-    <sortCondition ref="C124:C369"/>
+    <sortCondition ref="C93:C369"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{4A662F09-79DB-4DFC-8DCE-ED6253CFBF34}" name="team_id"/>
@@ -3143,8 +3143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N369"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="K130" sqref="K130"/>
+    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
+      <selection activeCell="C278" sqref="C278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3373,7 +3373,7 @@
         <v>211</v>
       </c>
       <c r="C9" t="s">
-        <v>211</v>
+        <v>559</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>543</v>
@@ -3393,77 +3393,77 @@
         <v>1605</v>
       </c>
       <c r="K9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>48</v>
+        <v>319</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>559</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>559</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>800</v>
+      </c>
+      <c r="F10" t="s">
+        <v>459</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>1605</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>247</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>239</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>239</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>617</v>
-      </c>
-      <c r="F11" t="s">
-        <v>444</v>
+        <v>48</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>2083</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>202</v>
+        <v>247</v>
       </c>
       <c r="B12" t="s">
-        <v>195</v>
+        <v>239</v>
       </c>
       <c r="C12" t="s">
-        <v>195</v>
+        <v>239</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>422</v>
+        <v>338</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F12" t="s">
-        <v>461</v>
+        <v>444</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -3471,7 +3471,7 @@
         <v>1</v>
       </c>
       <c r="J12">
-        <v>2549</v>
+        <v>2083</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -3479,22 +3479,22 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>221</v>
+        <v>202</v>
       </c>
       <c r="B13" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="C13" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>521</v>
+        <v>422</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="F13" t="s">
-        <v>447</v>
+        <v>461</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -3502,7 +3502,7 @@
         <v>1</v>
       </c>
       <c r="J13">
-        <v>1619</v>
+        <v>2549</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -3510,19 +3510,19 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>196</v>
+        <v>221</v>
       </c>
       <c r="B14" t="s">
-        <v>189</v>
+        <v>214</v>
       </c>
       <c r="C14" t="s">
-        <v>189</v>
+        <v>214</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>801</v>
+        <v>614</v>
       </c>
       <c r="F14" t="s">
         <v>447</v>
@@ -3533,7 +3533,7 @@
         <v>1</v>
       </c>
       <c r="J14">
-        <v>2049</v>
+        <v>1619</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -3541,72 +3541,72 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>277</v>
+        <v>196</v>
       </c>
       <c r="B15" t="s">
-        <v>265</v>
+        <v>189</v>
       </c>
       <c r="C15" t="s">
-        <v>265</v>
+        <v>189</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>801</v>
+      </c>
+      <c r="F15" t="s">
+        <v>447</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>2049</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>8</v>
+        <v>277</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>265</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>619</v>
-      </c>
-      <c r="F16" t="s">
-        <v>448</v>
+        <v>265</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>3037</v>
-      </c>
-      <c r="K16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>206</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>199</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>199</v>
+        <v>8</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>424</v>
+        <v>314</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="F17" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
@@ -3614,7 +3614,7 @@
         <v>1</v>
       </c>
       <c r="J17">
-        <v>2396</v>
+        <v>3037</v>
       </c>
       <c r="K17">
         <v>1</v>
@@ -3622,122 +3622,122 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>288</v>
+        <v>206</v>
       </c>
       <c r="B18" t="s">
-        <v>276</v>
+        <v>199</v>
       </c>
       <c r="C18" t="s">
-        <v>276</v>
+        <v>199</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>620</v>
+      </c>
+      <c r="F18" t="s">
+        <v>444</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>2396</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>53</v>
+        <v>288</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>276</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>621</v>
-      </c>
-      <c r="F19" t="s">
-        <v>447</v>
+        <v>276</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19">
-        <v>2369</v>
-      </c>
-      <c r="K19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>52</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="F20" t="s">
+        <v>447</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>2369</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>622</v>
-      </c>
-      <c r="F21" t="s">
-        <v>453</v>
+        <v>49</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21">
-        <v>2544</v>
-      </c>
-      <c r="K21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>449</v>
+        <v>315</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F22" t="s">
-        <v>444</v>
+        <v>453</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -3745,7 +3745,7 @@
         <v>1</v>
       </c>
       <c r="J22">
-        <v>2826</v>
+        <v>2544</v>
       </c>
       <c r="K22">
         <v>1</v>
@@ -3753,72 +3753,72 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>315</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>303</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>303</v>
+        <v>9</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>623</v>
+      </c>
+      <c r="F23" t="s">
+        <v>444</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23">
-        <v>0</v>
+        <v>2826</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>208</v>
+        <v>315</v>
       </c>
       <c r="B24" t="s">
-        <v>201</v>
+        <v>303</v>
       </c>
       <c r="C24" t="s">
-        <v>201</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>426</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>624</v>
-      </c>
-      <c r="F24" t="s">
-        <v>444</v>
+        <v>303</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24">
-        <v>2584</v>
-      </c>
-      <c r="K24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>189</v>
+        <v>208</v>
       </c>
       <c r="B25" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="C25" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>411</v>
+        <v>426</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F25" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
@@ -3826,7 +3826,7 @@
         <v>1</v>
       </c>
       <c r="J25">
-        <v>1934</v>
+        <v>2584</v>
       </c>
       <c r="K25">
         <v>1</v>
@@ -3834,22 +3834,22 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="B26" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="C26" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>513</v>
+        <v>411</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="F26" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -3857,7 +3857,7 @@
         <v>1</v>
       </c>
       <c r="J26">
-        <v>2224</v>
+        <v>1934</v>
       </c>
       <c r="K26">
         <v>1</v>
@@ -3865,19 +3865,19 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="B27" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="C27" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>419</v>
+        <v>513</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>626</v>
+        <v>631</v>
       </c>
       <c r="F27" t="s">
         <v>453</v>
@@ -3888,7 +3888,7 @@
         <v>1</v>
       </c>
       <c r="J27">
-        <v>1908</v>
+        <v>2224</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -3896,119 +3896,119 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>301</v>
+        <v>197</v>
       </c>
       <c r="B28" t="s">
-        <v>289</v>
+        <v>190</v>
       </c>
       <c r="C28" t="s">
-        <v>289</v>
+        <v>190</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>626</v>
+      </c>
+      <c r="F28" t="s">
+        <v>453</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28">
-        <v>0</v>
+        <v>1908</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>70</v>
+        <v>301</v>
       </c>
       <c r="B29" t="s">
-        <v>68</v>
+        <v>289</v>
       </c>
       <c r="C29" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>639</v>
-      </c>
-      <c r="F29" t="s">
-        <v>447</v>
+        <v>289</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29">
-        <v>2162</v>
-      </c>
-      <c r="K29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="B30" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="C30" t="s">
-        <v>27</v>
+        <v>68</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>639</v>
+      </c>
+      <c r="F30" t="s">
+        <v>447</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30">
-        <v>0</v>
+        <v>2162</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>546</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>633</v>
-      </c>
-      <c r="F31" t="s">
-        <v>444</v>
+        <v>27</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31">
-        <v>2455</v>
-      </c>
-      <c r="K31">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="B32" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>318</v>
+        <v>546</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>628</v>
+        <v>633</v>
       </c>
       <c r="F32" t="s">
         <v>444</v>
@@ -4019,7 +4019,7 @@
         <v>1</v>
       </c>
       <c r="J32">
-        <v>2735</v>
+        <v>2455</v>
       </c>
       <c r="K32">
         <v>1</v>
@@ -4027,32 +4027,30 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>320</v>
+        <v>12</v>
       </c>
       <c r="B33" t="s">
-        <v>560</v>
+        <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>212</v>
+        <v>12</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>520</v>
+        <v>318</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>805</v>
+        <v>628</v>
       </c>
       <c r="F33" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="G33" s="4"/>
-      <c r="H33" s="4">
-        <v>26815</v>
-      </c>
+      <c r="H33" s="4"/>
       <c r="I33" t="b">
         <v>1</v>
       </c>
       <c r="J33">
-        <v>2032</v>
+        <v>2735</v>
       </c>
       <c r="K33">
         <v>1</v>
@@ -4060,10 +4058,10 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>219</v>
+        <v>320</v>
       </c>
       <c r="B34" t="s">
-        <v>212</v>
+        <v>560</v>
       </c>
       <c r="C34" t="s">
         <v>212</v>
@@ -4072,15 +4070,15 @@
         <v>520</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>634</v>
+        <v>805</v>
       </c>
       <c r="F34" t="s">
         <v>447</v>
       </c>
-      <c r="G34" s="4">
-        <v>26816</v>
-      </c>
-      <c r="H34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4">
+        <v>26815</v>
+      </c>
       <c r="I34" t="b">
         <v>1</v>
       </c>
@@ -4088,48 +4086,48 @@
         <v>2032</v>
       </c>
       <c r="K34">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>322</v>
+        <v>219</v>
       </c>
       <c r="B35" t="s">
-        <v>562</v>
+        <v>212</v>
       </c>
       <c r="C35" t="s">
-        <v>147</v>
+        <v>212</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>398</v>
+        <v>520</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>668</v>
+        <v>634</v>
       </c>
       <c r="F35" t="s">
-        <v>461</v>
-      </c>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4">
-        <v>21861</v>
-      </c>
+        <v>447</v>
+      </c>
+      <c r="G35" s="4">
+        <v>26816</v>
+      </c>
+      <c r="H35" s="4"/>
       <c r="I35" t="b">
         <v>1</v>
       </c>
       <c r="J35">
-        <v>2266</v>
+        <v>2032</v>
       </c>
       <c r="K35">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B36" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C36" t="s">
         <v>147</v>
@@ -4138,16 +4136,14 @@
         <v>398</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>629</v>
+        <v>668</v>
       </c>
       <c r="F36" t="s">
         <v>461</v>
       </c>
-      <c r="G36" s="4">
-        <v>21862</v>
-      </c>
+      <c r="G36" s="4"/>
       <c r="H36" s="4">
-        <v>27727</v>
+        <v>21861</v>
       </c>
       <c r="I36" t="b">
         <v>1</v>
@@ -4156,15 +4152,15 @@
         <v>2266</v>
       </c>
       <c r="K36">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>152</v>
+        <v>321</v>
       </c>
       <c r="B37" t="s">
-        <v>147</v>
+        <v>561</v>
       </c>
       <c r="C37" t="s">
         <v>147</v>
@@ -4179,9 +4175,11 @@
         <v>461</v>
       </c>
       <c r="G37" s="4">
-        <v>27728</v>
-      </c>
-      <c r="H37" s="4"/>
+        <v>21862</v>
+      </c>
+      <c r="H37" s="4">
+        <v>27727</v>
+      </c>
       <c r="I37" t="b">
         <v>1</v>
       </c>
@@ -4189,58 +4187,60 @@
         <v>2266</v>
       </c>
       <c r="K37">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="B38" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="C38" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="F38" t="s">
-        <v>447</v>
-      </c>
-      <c r="G38" s="4"/>
+        <v>461</v>
+      </c>
+      <c r="G38" s="4">
+        <v>27728</v>
+      </c>
       <c r="H38" s="4"/>
       <c r="I38" t="b">
         <v>1</v>
       </c>
       <c r="J38">
-        <v>2120</v>
+        <v>2266</v>
       </c>
       <c r="K38">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>216</v>
+        <v>175</v>
       </c>
       <c r="B39" t="s">
-        <v>209</v>
+        <v>169</v>
       </c>
       <c r="C39" t="s">
-        <v>209</v>
+        <v>169</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>433</v>
+        <v>408</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="F39" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
@@ -4248,7 +4248,7 @@
         <v>1</v>
       </c>
       <c r="J39">
-        <v>1625</v>
+        <v>2120</v>
       </c>
       <c r="K39">
         <v>1</v>
@@ -4256,80 +4256,80 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>312</v>
+        <v>216</v>
       </c>
       <c r="B40" t="s">
-        <v>300</v>
+        <v>209</v>
       </c>
       <c r="C40" t="s">
-        <v>300</v>
+        <v>209</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>632</v>
+      </c>
+      <c r="F40" t="s">
+        <v>453</v>
       </c>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
       <c r="I40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40">
-        <v>0</v>
+        <v>1625</v>
+      </c>
+      <c r="K40">
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>63</v>
+        <v>312</v>
       </c>
       <c r="B41" t="s">
-        <v>61</v>
+        <v>300</v>
       </c>
       <c r="C41" t="s">
-        <v>61</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>635</v>
-      </c>
-      <c r="F41" t="s">
-        <v>448</v>
+        <v>300</v>
       </c>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
       <c r="I41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41">
-        <v>2413</v>
-      </c>
-      <c r="K41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>281</v>
+        <v>63</v>
       </c>
       <c r="B42" t="s">
-        <v>269</v>
+        <v>61</v>
       </c>
       <c r="C42" t="s">
-        <v>269</v>
+        <v>61</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>443</v>
+        <v>349</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F42" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
       <c r="I42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42">
-        <v>1791</v>
+        <v>2413</v>
       </c>
       <c r="K42">
         <v>1</v>
@@ -4338,30 +4338,30 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>244</v>
+        <v>281</v>
       </c>
       <c r="B43" t="s">
-        <v>236</v>
+        <v>269</v>
       </c>
       <c r="C43" t="s">
-        <v>236</v>
+        <v>269</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>531</v>
+        <v>443</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>804</v>
+        <v>636</v>
       </c>
       <c r="F43" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
       <c r="I43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43">
-        <v>2648</v>
+        <v>1791</v>
       </c>
       <c r="K43">
         <v>1</v>
@@ -4369,22 +4369,22 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>186</v>
+        <v>244</v>
       </c>
       <c r="B44" t="s">
-        <v>180</v>
+        <v>236</v>
       </c>
       <c r="C44" t="s">
-        <v>180</v>
+        <v>236</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>413</v>
+        <v>531</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>637</v>
+        <v>804</v>
       </c>
       <c r="F44" t="s">
-        <v>461</v>
+        <v>444</v>
       </c>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
@@ -4392,7 +4392,7 @@
         <v>1</v>
       </c>
       <c r="J44">
-        <v>2043</v>
+        <v>2648</v>
       </c>
       <c r="K44">
         <v>1</v>
@@ -4400,22 +4400,22 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>26</v>
+        <v>186</v>
       </c>
       <c r="B45" t="s">
-        <v>26</v>
+        <v>180</v>
       </c>
       <c r="C45" t="s">
-        <v>26</v>
+        <v>180</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>328</v>
+        <v>413</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="F45" t="s">
-        <v>448</v>
+        <v>461</v>
       </c>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
@@ -4423,7 +4423,7 @@
         <v>1</v>
       </c>
       <c r="J45">
-        <v>2960</v>
+        <v>2043</v>
       </c>
       <c r="K45">
         <v>1</v>
@@ -4431,22 +4431,22 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>222</v>
+        <v>26</v>
       </c>
       <c r="B46" t="s">
-        <v>215</v>
+        <v>26</v>
       </c>
       <c r="C46" t="s">
-        <v>215</v>
+        <v>26</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>522</v>
+        <v>328</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>864</v>
+        <v>638</v>
       </c>
       <c r="F46" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
@@ -4454,7 +4454,7 @@
         <v>1</v>
       </c>
       <c r="J46">
-        <v>1731</v>
+        <v>2960</v>
       </c>
       <c r="K46">
         <v>1</v>
@@ -4462,72 +4462,72 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>40</v>
+        <v>222</v>
       </c>
       <c r="B47" t="s">
-        <v>40</v>
+        <v>215</v>
       </c>
       <c r="C47" t="s">
-        <v>40</v>
+        <v>215</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>864</v>
+      </c>
+      <c r="F47" t="s">
+        <v>447</v>
       </c>
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
       <c r="I47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J47">
-        <v>0</v>
+        <v>1731</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>190</v>
+        <v>40</v>
       </c>
       <c r="B48" t="s">
-        <v>184</v>
+        <v>40</v>
       </c>
       <c r="C48" t="s">
-        <v>184</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>640</v>
-      </c>
-      <c r="F48" t="s">
-        <v>453</v>
+        <v>40</v>
       </c>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
       <c r="I48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48">
-        <v>1667</v>
-      </c>
-      <c r="K48">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>55</v>
+        <v>190</v>
       </c>
       <c r="B49" t="s">
-        <v>54</v>
+        <v>184</v>
       </c>
       <c r="C49" t="s">
-        <v>54</v>
+        <v>184</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>343</v>
+        <v>416</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="F49" t="s">
-        <v>444</v>
+        <v>453</v>
       </c>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
@@ -4535,7 +4535,7 @@
         <v>1</v>
       </c>
       <c r="J49">
-        <v>2094</v>
+        <v>1667</v>
       </c>
       <c r="K49">
         <v>1</v>
@@ -4543,32 +4543,30 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>323</v>
+        <v>55</v>
       </c>
       <c r="B50" t="s">
-        <v>563</v>
+        <v>54</v>
       </c>
       <c r="C50" t="s">
-        <v>153</v>
+        <v>54</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>500</v>
+        <v>343</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>803</v>
+        <v>641</v>
       </c>
       <c r="F50" t="s">
-        <v>461</v>
+        <v>444</v>
       </c>
       <c r="G50" s="4"/>
-      <c r="H50" s="4">
-        <v>30897</v>
-      </c>
+      <c r="H50" s="4"/>
       <c r="I50" t="b">
         <v>1</v>
       </c>
       <c r="J50">
-        <v>2351</v>
+        <v>2094</v>
       </c>
       <c r="K50">
         <v>1</v>
@@ -4576,10 +4574,10 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>158</v>
+        <v>323</v>
       </c>
       <c r="B51" t="s">
-        <v>153</v>
+        <v>563</v>
       </c>
       <c r="C51" t="s">
         <v>153</v>
@@ -4588,15 +4586,15 @@
         <v>500</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="F51" t="s">
         <v>461</v>
       </c>
-      <c r="G51" s="4">
-        <v>30898</v>
-      </c>
-      <c r="H51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4">
+        <v>30897</v>
+      </c>
       <c r="I51" t="b">
         <v>1</v>
       </c>
@@ -4604,48 +4602,48 @@
         <v>2351</v>
       </c>
       <c r="K51">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>324</v>
+        <v>158</v>
       </c>
       <c r="B52" t="s">
-        <v>564</v>
+        <v>153</v>
       </c>
       <c r="C52" t="s">
-        <v>131</v>
+        <v>153</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>628</v>
+        <v>802</v>
       </c>
       <c r="F52" t="s">
         <v>461</v>
       </c>
-      <c r="G52" s="4"/>
-      <c r="H52" s="4">
-        <v>22827</v>
-      </c>
+      <c r="G52" s="4">
+        <v>30898</v>
+      </c>
+      <c r="H52" s="4"/>
       <c r="I52" t="b">
         <v>1</v>
       </c>
       <c r="J52">
-        <v>2157</v>
+        <v>2351</v>
       </c>
       <c r="K52">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>136</v>
+        <v>324</v>
       </c>
       <c r="B53" t="s">
-        <v>131</v>
+        <v>564</v>
       </c>
       <c r="C53" t="s">
         <v>131</v>
@@ -4654,15 +4652,15 @@
         <v>504</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="F53" t="s">
         <v>461</v>
       </c>
-      <c r="G53" s="4">
-        <v>22828</v>
-      </c>
-      <c r="H53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4">
+        <v>22827</v>
+      </c>
       <c r="I53" t="b">
         <v>1</v>
       </c>
@@ -4670,50 +4668,48 @@
         <v>2157</v>
       </c>
       <c r="K53">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>325</v>
+        <v>136</v>
       </c>
       <c r="B54" t="s">
-        <v>565</v>
+        <v>131</v>
       </c>
       <c r="C54" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>393</v>
+        <v>504</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>806</v>
+        <v>627</v>
       </c>
       <c r="F54" t="s">
-        <v>453</v>
+        <v>461</v>
       </c>
       <c r="G54" s="4">
-        <v>25645</v>
-      </c>
-      <c r="H54" s="4">
-        <v>27501</v>
-      </c>
+        <v>22828</v>
+      </c>
+      <c r="H54" s="4"/>
       <c r="I54" t="b">
         <v>1</v>
       </c>
       <c r="J54">
-        <v>2004</v>
+        <v>2157</v>
       </c>
       <c r="K54">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>138</v>
+        <v>325</v>
       </c>
       <c r="B55" t="s">
-        <v>133</v>
+        <v>565</v>
       </c>
       <c r="C55" t="s">
         <v>133</v>
@@ -4722,13 +4718,17 @@
         <v>393</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>642</v>
+        <v>806</v>
       </c>
       <c r="F55" t="s">
         <v>453</v>
       </c>
-      <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
+      <c r="G55" s="4">
+        <v>25645</v>
+      </c>
+      <c r="H55" s="4">
+        <v>27501</v>
+      </c>
       <c r="I55" t="b">
         <v>1</v>
       </c>
@@ -4736,27 +4736,27 @@
         <v>2004</v>
       </c>
       <c r="K55">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="B56" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="C56" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>497</v>
+        <v>393</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="F56" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
@@ -4764,30 +4764,30 @@
         <v>1</v>
       </c>
       <c r="J56">
-        <v>2546</v>
+        <v>2004</v>
       </c>
       <c r="K56">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>6</v>
+        <v>154</v>
       </c>
       <c r="B57" t="s">
-        <v>6</v>
+        <v>149</v>
       </c>
       <c r="C57" t="s">
-        <v>6</v>
+        <v>149</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>312</v>
+        <v>497</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
       <c r="F57" t="s">
-        <v>447</v>
+        <v>461</v>
       </c>
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
@@ -4795,7 +4795,7 @@
         <v>1</v>
       </c>
       <c r="J57">
-        <v>2524</v>
+        <v>2546</v>
       </c>
       <c r="K57">
         <v>1</v>
@@ -4803,82 +4803,94 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>245</v>
+        <v>6</v>
       </c>
       <c r="B58" t="s">
-        <v>237</v>
+        <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>237</v>
+        <v>6</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>643</v>
+      </c>
+      <c r="F58" t="s">
+        <v>447</v>
       </c>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J58">
-        <v>0</v>
+        <v>2524</v>
+      </c>
+      <c r="K58">
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>153</v>
+        <v>245</v>
       </c>
       <c r="B59" t="s">
-        <v>148</v>
+        <v>237</v>
       </c>
       <c r="C59" t="s">
-        <v>148</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>496</v>
-      </c>
-      <c r="E59" s="7" t="s">
-        <v>813</v>
-      </c>
-      <c r="F59" t="s">
-        <v>461</v>
+        <v>237</v>
       </c>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J59">
-        <v>2238</v>
-      </c>
-      <c r="K59">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>305</v>
+        <v>153</v>
       </c>
       <c r="B60" t="s">
-        <v>293</v>
+        <v>148</v>
       </c>
       <c r="C60" t="s">
-        <v>293</v>
+        <v>148</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>813</v>
+      </c>
+      <c r="F60" t="s">
+        <v>461</v>
       </c>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
       <c r="I60" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J60">
-        <v>0</v>
+        <v>2238</v>
+      </c>
+      <c r="K60">
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>23</v>
+        <v>305</v>
       </c>
       <c r="B61" t="s">
-        <v>23</v>
+        <v>293</v>
       </c>
       <c r="C61" t="s">
-        <v>23</v>
+        <v>293</v>
       </c>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
@@ -4891,63 +4903,49 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>220</v>
+        <v>23</v>
       </c>
       <c r="B62" t="s">
-        <v>213</v>
+        <v>23</v>
       </c>
       <c r="C62" t="s">
-        <v>213</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>435</v>
-      </c>
-      <c r="E62" s="7" t="s">
-        <v>807</v>
-      </c>
-      <c r="F62" t="s">
-        <v>447</v>
+        <v>23</v>
       </c>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
       <c r="I62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J62">
-        <v>1874</v>
-      </c>
-      <c r="K62">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>326</v>
+        <v>220</v>
       </c>
       <c r="B63" t="s">
-        <v>566</v>
+        <v>213</v>
       </c>
       <c r="C63" t="s">
-        <v>150</v>
+        <v>213</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>498</v>
+        <v>435</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>668</v>
+        <v>807</v>
       </c>
       <c r="F63" t="s">
-        <v>461</v>
+        <v>447</v>
       </c>
       <c r="G63" s="4"/>
-      <c r="H63" s="4">
-        <v>21185</v>
-      </c>
+      <c r="H63" s="4"/>
       <c r="I63" t="b">
         <v>1</v>
       </c>
       <c r="J63">
-        <v>2184</v>
+        <v>1874</v>
       </c>
       <c r="K63">
         <v>1</v>
@@ -4955,10 +4953,10 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>155</v>
+        <v>326</v>
       </c>
       <c r="B64" t="s">
-        <v>150</v>
+        <v>566</v>
       </c>
       <c r="C64" t="s">
         <v>150</v>
@@ -4967,15 +4965,15 @@
         <v>498</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>815</v>
+        <v>668</v>
       </c>
       <c r="F64" t="s">
         <v>461</v>
       </c>
-      <c r="G64" s="4">
-        <v>21186</v>
-      </c>
-      <c r="H64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4">
+        <v>21185</v>
+      </c>
       <c r="I64" t="b">
         <v>1</v>
       </c>
@@ -4983,76 +4981,87 @@
         <v>2184</v>
       </c>
       <c r="K64">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>46</v>
+        <v>155</v>
       </c>
       <c r="B65" t="s">
-        <v>46</v>
+        <v>150</v>
       </c>
       <c r="C65" t="s">
-        <v>46</v>
-      </c>
-      <c r="G65" s="4"/>
+        <v>150</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>815</v>
+      </c>
+      <c r="F65" t="s">
+        <v>461</v>
+      </c>
+      <c r="G65" s="4">
+        <v>21186</v>
+      </c>
       <c r="H65" s="4"/>
       <c r="I65" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J65">
-        <v>0</v>
+        <v>2184</v>
+      </c>
+      <c r="K65">
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>174</v>
+        <v>46</v>
       </c>
       <c r="B66" t="s">
-        <v>168</v>
+        <v>46</v>
       </c>
       <c r="C66" t="s">
-        <v>168</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E66" s="7" t="s">
-        <v>645</v>
-      </c>
-      <c r="F66" t="s">
-        <v>461</v>
+        <v>46</v>
       </c>
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
       <c r="I66" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J66">
-        <v>2104</v>
-      </c>
-      <c r="K66">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>296</v>
+        <v>174</v>
       </c>
       <c r="B67" t="s">
-        <v>284</v>
+        <v>168</v>
       </c>
       <c r="C67" t="s">
-        <v>284</v>
+        <v>168</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>645</v>
+      </c>
+      <c r="F67" t="s">
+        <v>461</v>
       </c>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
       <c r="I67" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J67">
-        <v>0</v>
+        <v>2104</v>
       </c>
       <c r="K67">
         <v>1</v>
@@ -5060,13 +5069,13 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="B68" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C68" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="G68" s="4"/>
       <c r="H68" s="4"/>
@@ -5076,56 +5085,47 @@
       <c r="J68">
         <v>0</v>
       </c>
+      <c r="K68">
+        <v>1</v>
+      </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>20</v>
+        <v>309</v>
       </c>
       <c r="B69" t="s">
-        <v>20</v>
+        <v>297</v>
       </c>
       <c r="C69" t="s">
-        <v>20</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="E69" s="7" t="s">
-        <v>646</v>
-      </c>
-      <c r="F69" t="s">
-        <v>448</v>
+        <v>297</v>
       </c>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
       <c r="I69" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J69">
-        <v>2453</v>
-      </c>
-      <c r="K69">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="B70" t="s">
-        <v>549</v>
+        <v>20</v>
       </c>
       <c r="C70" t="s">
-        <v>549</v>
+        <v>20</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>460</v>
+        <v>323</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>751</v>
+        <v>646</v>
       </c>
       <c r="F70" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
@@ -5133,7 +5133,7 @@
         <v>1</v>
       </c>
       <c r="J70">
-        <v>2539</v>
+        <v>2453</v>
       </c>
       <c r="K70">
         <v>1</v>
@@ -5141,22 +5141,22 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="B71" t="s">
-        <v>82</v>
+        <v>549</v>
       </c>
       <c r="C71" t="s">
-        <v>82</v>
+        <v>549</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>363</v>
+        <v>460</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>649</v>
+        <v>751</v>
       </c>
       <c r="F71" t="s">
-        <v>448</v>
+        <v>453</v>
       </c>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
@@ -5164,7 +5164,7 @@
         <v>1</v>
       </c>
       <c r="J71">
-        <v>2447</v>
+        <v>2539</v>
       </c>
       <c r="K71">
         <v>1</v>
@@ -5172,22 +5172,22 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>273</v>
+        <v>84</v>
       </c>
       <c r="B72" t="s">
-        <v>261</v>
+        <v>82</v>
       </c>
       <c r="C72" t="s">
-        <v>261</v>
+        <v>82</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>442</v>
+        <v>363</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="F72" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
@@ -5195,7 +5195,7 @@
         <v>1</v>
       </c>
       <c r="J72">
-        <v>1928</v>
+        <v>2447</v>
       </c>
       <c r="K72">
         <v>1</v>
@@ -5204,32 +5204,30 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>327</v>
+        <v>273</v>
       </c>
       <c r="B73" t="s">
-        <v>567</v>
+        <v>261</v>
       </c>
       <c r="C73" t="s">
-        <v>155</v>
+        <v>261</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>502</v>
+        <v>442</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>668</v>
+        <v>650</v>
       </c>
       <c r="F73" t="s">
         <v>461</v>
       </c>
       <c r="G73" s="4"/>
-      <c r="H73" s="4">
-        <v>21974</v>
-      </c>
+      <c r="H73" s="4"/>
       <c r="I73" t="b">
         <v>1</v>
       </c>
       <c r="J73">
-        <v>2432</v>
+        <v>1928</v>
       </c>
       <c r="K73">
         <v>1</v>
@@ -5237,10 +5235,10 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>160</v>
+        <v>327</v>
       </c>
       <c r="B74" t="s">
-        <v>155</v>
+        <v>567</v>
       </c>
       <c r="C74" t="s">
         <v>155</v>
@@ -5249,15 +5247,15 @@
         <v>502</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>644</v>
+        <v>668</v>
       </c>
       <c r="F74" t="s">
         <v>461</v>
       </c>
-      <c r="G74" s="4">
-        <v>21975</v>
-      </c>
-      <c r="H74" s="4"/>
+      <c r="G74" s="4"/>
+      <c r="H74" s="4">
+        <v>21974</v>
+      </c>
       <c r="I74" t="b">
         <v>1</v>
       </c>
@@ -5265,118 +5263,132 @@
         <v>2432</v>
       </c>
       <c r="K74">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>191</v>
+        <v>160</v>
       </c>
       <c r="B75" t="s">
-        <v>185</v>
+        <v>155</v>
       </c>
       <c r="C75" t="s">
-        <v>185</v>
+        <v>155</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>514</v>
+        <v>502</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>812</v>
+        <v>644</v>
       </c>
       <c r="F75" t="s">
-        <v>459</v>
-      </c>
-      <c r="G75" s="4"/>
+        <v>461</v>
+      </c>
+      <c r="G75" s="4">
+        <v>21975</v>
+      </c>
       <c r="H75" s="4"/>
       <c r="I75" t="b">
         <v>1</v>
       </c>
       <c r="J75">
-        <v>1718</v>
+        <v>2432</v>
       </c>
       <c r="K75">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="B76" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="C76" t="s">
-        <v>176</v>
+        <v>185</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>812</v>
+      </c>
+      <c r="F76" t="s">
+        <v>459</v>
       </c>
       <c r="G76" s="4"/>
       <c r="H76" s="4"/>
       <c r="I76" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J76">
-        <v>0</v>
+        <v>1718</v>
+      </c>
+      <c r="K76">
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>33</v>
+        <v>182</v>
       </c>
       <c r="B77" t="s">
-        <v>33</v>
+        <v>176</v>
       </c>
       <c r="C77" t="s">
-        <v>33</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="E77" s="7" t="s">
-        <v>814</v>
-      </c>
-      <c r="F77" t="s">
-        <v>447</v>
+        <v>176</v>
       </c>
       <c r="G77" s="4"/>
       <c r="H77" s="4"/>
       <c r="I77" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J77">
-        <v>2616</v>
-      </c>
-      <c r="K77">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>292</v>
+        <v>33</v>
       </c>
       <c r="B78" t="s">
-        <v>280</v>
+        <v>33</v>
       </c>
       <c r="C78" t="s">
-        <v>280</v>
+        <v>33</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="E78" s="7" t="s">
+        <v>814</v>
+      </c>
+      <c r="F78" t="s">
+        <v>447</v>
       </c>
       <c r="G78" s="4"/>
       <c r="H78" s="4"/>
       <c r="I78" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J78">
-        <v>0</v>
+        <v>2616</v>
+      </c>
+      <c r="K78">
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>270</v>
+        <v>292</v>
       </c>
       <c r="B79" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="C79" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="G79" s="4"/>
       <c r="H79" s="4"/>
@@ -5389,53 +5401,41 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>92</v>
+        <v>270</v>
       </c>
       <c r="B80" t="s">
-        <v>90</v>
+        <v>258</v>
       </c>
       <c r="C80" t="s">
-        <v>90</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>366</v>
-      </c>
-      <c r="E80" s="7" t="s">
-        <v>651</v>
-      </c>
-      <c r="F80" t="s">
-        <v>444</v>
+        <v>258</v>
       </c>
       <c r="G80" s="4"/>
       <c r="H80" s="4"/>
       <c r="I80" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J80">
-        <v>2890</v>
-      </c>
-      <c r="K80">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="B81" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="C81" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>358</v>
+        <v>366</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="F81" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="G81" s="4"/>
       <c r="H81" s="4"/>
@@ -5443,7 +5443,7 @@
         <v>1</v>
       </c>
       <c r="J81">
-        <v>2317</v>
+        <v>2890</v>
       </c>
       <c r="K81">
         <v>1</v>
@@ -5451,32 +5451,30 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>328</v>
+        <v>76</v>
       </c>
       <c r="B82" t="s">
-        <v>568</v>
+        <v>74</v>
       </c>
       <c r="C82" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>451</v>
+        <v>358</v>
       </c>
       <c r="E82" s="7" t="s">
-        <v>835</v>
+        <v>652</v>
       </c>
       <c r="F82" t="s">
         <v>447</v>
       </c>
       <c r="G82" s="4"/>
-      <c r="H82" s="4">
-        <v>40468</v>
-      </c>
+      <c r="H82" s="4"/>
       <c r="I82" t="b">
         <v>1</v>
       </c>
       <c r="J82">
-        <v>2328</v>
+        <v>2317</v>
       </c>
       <c r="K82">
         <v>1</v>
@@ -5484,27 +5482,27 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>54</v>
+        <v>328</v>
       </c>
       <c r="B83" t="s">
-        <v>53</v>
+        <v>568</v>
       </c>
       <c r="C83" t="s">
         <v>53</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>342</v>
+        <v>451</v>
       </c>
       <c r="E83" s="7" t="s">
-        <v>816</v>
+        <v>835</v>
       </c>
       <c r="F83" t="s">
         <v>447</v>
       </c>
-      <c r="G83" s="4">
-        <v>40469</v>
-      </c>
-      <c r="H83" s="4"/>
+      <c r="G83" s="4"/>
+      <c r="H83" s="4">
+        <v>40468</v>
+      </c>
       <c r="I83" t="b">
         <v>1</v>
       </c>
@@ -5512,68 +5510,68 @@
         <v>2328</v>
       </c>
       <c r="K83">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>115</v>
+        <v>54</v>
       </c>
       <c r="B84" t="s">
-        <v>111</v>
+        <v>53</v>
       </c>
       <c r="C84" t="s">
-        <v>111</v>
+        <v>53</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>379</v>
+        <v>342</v>
       </c>
       <c r="E84" s="7" t="s">
-        <v>653</v>
+        <v>816</v>
       </c>
       <c r="F84" t="s">
-        <v>444</v>
-      </c>
-      <c r="G84" s="4"/>
+        <v>447</v>
+      </c>
+      <c r="G84" s="4">
+        <v>40469</v>
+      </c>
       <c r="H84" s="4"/>
       <c r="I84" t="b">
         <v>1</v>
       </c>
       <c r="J84">
-        <v>2273</v>
+        <v>2328</v>
       </c>
       <c r="K84">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>329</v>
+        <v>115</v>
       </c>
       <c r="B85" t="s">
-        <v>569</v>
+        <v>111</v>
       </c>
       <c r="C85" t="s">
-        <v>550</v>
+        <v>111</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>317</v>
+        <v>379</v>
       </c>
       <c r="E85" s="7" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="F85" t="s">
         <v>444</v>
       </c>
       <c r="G85" s="4"/>
-      <c r="H85" s="4">
-        <v>6875</v>
-      </c>
+      <c r="H85" s="4"/>
       <c r="I85" t="b">
         <v>1</v>
       </c>
       <c r="J85">
-        <v>2892</v>
+        <v>2273</v>
       </c>
       <c r="K85">
         <v>1</v>
@@ -5581,10 +5579,10 @@
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B86" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C86" t="s">
         <v>550</v>
@@ -5593,16 +5591,14 @@
         <v>317</v>
       </c>
       <c r="E86" s="7" t="s">
-        <v>817</v>
+        <v>654</v>
       </c>
       <c r="F86" t="s">
         <v>444</v>
       </c>
-      <c r="G86" s="4">
-        <v>14320</v>
-      </c>
+      <c r="G86" s="4"/>
       <c r="H86" s="4">
-        <v>16565</v>
+        <v>6875</v>
       </c>
       <c r="I86" t="b">
         <v>1</v>
@@ -5611,16 +5607,16 @@
         <v>2892</v>
       </c>
       <c r="K86">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N86" s="5"/>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>11</v>
+        <v>330</v>
       </c>
       <c r="B87" t="s">
-        <v>11</v>
+        <v>570</v>
       </c>
       <c r="C87" t="s">
         <v>550</v>
@@ -5629,14 +5625,16 @@
         <v>317</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>655</v>
+        <v>817</v>
       </c>
       <c r="F87" t="s">
         <v>444</v>
       </c>
-      <c r="G87" s="4"/>
+      <c r="G87" s="4">
+        <v>14320</v>
+      </c>
       <c r="H87" s="4">
-        <v>34334</v>
+        <v>16565</v>
       </c>
       <c r="I87" t="b">
         <v>1</v>
@@ -5645,15 +5643,15 @@
         <v>2892</v>
       </c>
       <c r="K87">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>240</v>
+        <v>11</v>
       </c>
       <c r="B88" t="s">
-        <v>550</v>
+        <v>11</v>
       </c>
       <c r="C88" t="s">
         <v>550</v>
@@ -5667,10 +5665,10 @@
       <c r="F88" t="s">
         <v>444</v>
       </c>
-      <c r="G88" s="4">
-        <v>34335</v>
-      </c>
-      <c r="H88" s="4"/>
+      <c r="G88" s="4"/>
+      <c r="H88" s="4">
+        <v>34334</v>
+      </c>
       <c r="I88" t="b">
         <v>1</v>
       </c>
@@ -5678,87 +5676,87 @@
         <v>2892</v>
       </c>
       <c r="K88">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>284</v>
+        <v>240</v>
       </c>
       <c r="B89" t="s">
-        <v>272</v>
+        <v>550</v>
       </c>
       <c r="C89" t="s">
-        <v>272</v>
-      </c>
-      <c r="G89" s="4"/>
+        <v>550</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>655</v>
+      </c>
+      <c r="F89" t="s">
+        <v>444</v>
+      </c>
+      <c r="G89" s="4">
+        <v>34335</v>
+      </c>
       <c r="H89" s="4"/>
       <c r="I89" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J89">
-        <v>0</v>
+        <v>2892</v>
+      </c>
+      <c r="K89">
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>25</v>
+        <v>284</v>
       </c>
       <c r="B90" t="s">
-        <v>25</v>
+        <v>272</v>
       </c>
       <c r="C90" t="s">
-        <v>25</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="E90" s="7" t="s">
-        <v>656</v>
-      </c>
-      <c r="F90" t="s">
-        <v>444</v>
+        <v>272</v>
       </c>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
       <c r="I90" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J90">
-        <v>2777</v>
-      </c>
-      <c r="K90">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>331</v>
+        <v>25</v>
       </c>
       <c r="B91" t="s">
-        <v>571</v>
+        <v>25</v>
       </c>
       <c r="C91" t="s">
-        <v>105</v>
+        <v>25</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>375</v>
+        <v>327</v>
       </c>
       <c r="E91" s="7" t="s">
-        <v>668</v>
+        <v>656</v>
       </c>
       <c r="F91" t="s">
-        <v>461</v>
+        <v>444</v>
       </c>
       <c r="G91" s="4"/>
-      <c r="H91" s="4">
-        <v>24657</v>
-      </c>
+      <c r="H91" s="4"/>
       <c r="I91" t="b">
         <v>1</v>
       </c>
       <c r="J91">
-        <v>1787</v>
+        <v>2777</v>
       </c>
       <c r="K91">
         <v>1</v>
@@ -5766,10 +5764,10 @@
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>108</v>
+        <v>331</v>
       </c>
       <c r="B92" t="s">
-        <v>105</v>
+        <v>571</v>
       </c>
       <c r="C92" t="s">
         <v>105</v>
@@ -5778,15 +5776,15 @@
         <v>375</v>
       </c>
       <c r="E92" s="7" t="s">
-        <v>657</v>
+        <v>668</v>
       </c>
       <c r="F92" t="s">
         <v>461</v>
       </c>
-      <c r="G92" s="4">
-        <v>24658</v>
-      </c>
-      <c r="H92" s="4"/>
+      <c r="G92" s="4"/>
+      <c r="H92" s="4">
+        <v>24657</v>
+      </c>
       <c r="I92" t="b">
         <v>1</v>
       </c>
@@ -5794,55 +5792,57 @@
         <v>1787</v>
       </c>
       <c r="K92">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="B93" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="C93" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>479</v>
+        <v>375</v>
       </c>
       <c r="E93" s="7" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="F93" t="s">
-        <v>447</v>
-      </c>
-      <c r="G93" s="4"/>
+        <v>461</v>
+      </c>
+      <c r="G93" s="4">
+        <v>24658</v>
+      </c>
       <c r="H93" s="4"/>
       <c r="I93" t="b">
         <v>1</v>
       </c>
       <c r="J93">
-        <v>2141</v>
+        <v>1787</v>
       </c>
       <c r="K93">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>114</v>
+        <v>74</v>
       </c>
       <c r="B94" t="s">
-        <v>110</v>
+        <v>72</v>
       </c>
       <c r="C94" t="s">
-        <v>110</v>
+        <v>72</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>357</v>
+        <v>479</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>818</v>
+        <v>658</v>
       </c>
       <c r="F94" t="s">
         <v>447</v>
@@ -5853,7 +5853,7 @@
         <v>1</v>
       </c>
       <c r="J94">
-        <v>2012</v>
+        <v>2141</v>
       </c>
       <c r="K94">
         <v>1</v>
@@ -5861,32 +5861,30 @@
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>333</v>
+        <v>114</v>
       </c>
       <c r="B95" t="s">
-        <v>573</v>
+        <v>110</v>
       </c>
       <c r="C95" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>503</v>
+        <v>357</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>809</v>
+        <v>818</v>
       </c>
       <c r="F95" t="s">
-        <v>461</v>
+        <v>447</v>
       </c>
       <c r="G95" s="4"/>
-      <c r="H95" s="4">
-        <v>22096</v>
-      </c>
+      <c r="H95" s="4"/>
       <c r="I95" t="b">
         <v>1</v>
       </c>
       <c r="J95">
-        <v>2520</v>
+        <v>2012</v>
       </c>
       <c r="K95">
         <v>1</v>
@@ -5894,10 +5892,10 @@
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B96" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C96" t="s">
         <v>107</v>
@@ -5906,16 +5904,14 @@
         <v>503</v>
       </c>
       <c r="E96" s="7" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="F96" t="s">
         <v>461</v>
       </c>
-      <c r="G96" s="4">
-        <v>22097</v>
-      </c>
+      <c r="G96" s="4"/>
       <c r="H96" s="4">
-        <v>23589</v>
+        <v>22096</v>
       </c>
       <c r="I96" t="b">
         <v>1</v>
@@ -5924,15 +5920,15 @@
         <v>2520</v>
       </c>
       <c r="K96">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B97" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="C97" t="s">
         <v>107</v>
@@ -5941,16 +5937,16 @@
         <v>503</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>648</v>
+        <v>810</v>
       </c>
       <c r="F97" t="s">
         <v>461</v>
       </c>
       <c r="G97" s="4">
-        <v>26233</v>
+        <v>22097</v>
       </c>
       <c r="H97" s="4">
-        <v>35565</v>
+        <v>23589</v>
       </c>
       <c r="I97" t="b">
         <v>1</v>
@@ -5959,15 +5955,15 @@
         <v>2520</v>
       </c>
       <c r="K97">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>110</v>
+        <v>332</v>
       </c>
       <c r="B98" t="s">
-        <v>107</v>
+        <v>572</v>
       </c>
       <c r="C98" t="s">
         <v>107</v>
@@ -5976,15 +5972,17 @@
         <v>503</v>
       </c>
       <c r="E98" s="7" t="s">
-        <v>811</v>
+        <v>648</v>
       </c>
       <c r="F98" t="s">
         <v>461</v>
       </c>
       <c r="G98" s="4">
-        <v>23590</v>
-      </c>
-      <c r="H98" s="4"/>
+        <v>26233</v>
+      </c>
+      <c r="H98" s="4">
+        <v>35565</v>
+      </c>
       <c r="I98" t="b">
         <v>1</v>
       </c>
@@ -5992,70 +5990,72 @@
         <v>2520</v>
       </c>
       <c r="K98">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="B99" t="s">
-        <v>551</v>
+        <v>107</v>
       </c>
       <c r="C99" t="s">
-        <v>551</v>
+        <v>107</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>484</v>
+        <v>503</v>
       </c>
       <c r="E99" s="7" t="s">
-        <v>822</v>
+        <v>811</v>
       </c>
       <c r="F99" t="s">
-        <v>444</v>
+        <v>461</v>
       </c>
       <c r="G99" s="4">
-        <v>18178</v>
-      </c>
-      <c r="H99" s="4">
-        <v>33148</v>
-      </c>
+        <v>23590</v>
+      </c>
+      <c r="H99" s="4"/>
       <c r="I99" t="b">
         <v>1</v>
       </c>
       <c r="J99">
-        <v>2839</v>
+        <v>2520</v>
       </c>
       <c r="K99">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>263</v>
+        <v>128</v>
       </c>
       <c r="B100" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C100" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>535</v>
+        <v>484</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>858</v>
+        <v>822</v>
       </c>
       <c r="F100" t="s">
-        <v>453</v>
-      </c>
-      <c r="G100" s="4"/>
-      <c r="H100" s="4"/>
+        <v>444</v>
+      </c>
+      <c r="G100" s="4">
+        <v>18178</v>
+      </c>
+      <c r="H100" s="4">
+        <v>33148</v>
+      </c>
       <c r="I100" t="b">
         <v>1</v>
       </c>
       <c r="J100">
-        <v>1723</v>
+        <v>2839</v>
       </c>
       <c r="K100">
         <v>1</v>
@@ -6063,21 +6063,33 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>319</v>
+        <v>263</v>
       </c>
       <c r="B101" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="C101" t="s">
-        <v>559</v>
+        <v>552</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>535</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>800</v>
+        <v>858</v>
+      </c>
+      <c r="F101" t="s">
+        <v>453</v>
       </c>
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
+      <c r="I101" t="b">
+        <v>1</v>
+      </c>
+      <c r="J101">
+        <v>1723</v>
+      </c>
       <c r="K101">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
@@ -11101,7 +11113,9 @@
       <c r="F277" t="s">
         <v>459</v>
       </c>
-      <c r="G277" s="4"/>
+      <c r="G277" s="4">
+        <v>35796</v>
+      </c>
       <c r="H277" s="4"/>
       <c r="I277" t="b">
         <v>1</v>
@@ -11110,7 +11124,7 @@
         <v>1532</v>
       </c>
       <c r="K277">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="278" spans="1:11" x14ac:dyDescent="0.25">
@@ -11133,7 +11147,9 @@
         <v>459</v>
       </c>
       <c r="G278" s="4"/>
-      <c r="H278" s="4"/>
+      <c r="H278" s="4">
+        <v>35795</v>
+      </c>
       <c r="I278" t="b">
         <v>1</v>
       </c>
@@ -11141,7 +11157,7 @@
         <v>1532</v>
       </c>
       <c r="K278">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="279" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>